<commit_message>
Adding test cases without relaoding HUB
</commit_message>
<xml_diff>
--- a/target/test-classes/com/rsystems/config/testdata.xlsx
+++ b/target/test-classes/com/rsystems/config/testdata.xlsx
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding comment Test1 in OR
</commit_message>
<xml_diff>
--- a/target/test-classes/com/rsystems/config/testdata.xlsx
+++ b/target/test-classes/com/rsystems/config/testdata.xlsx
@@ -4,25 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
-    <sheet name="testdata" sheetId="3" r:id="rId2"/>
-    <sheet name="system" sheetId="4" r:id="rId3"/>
+    <sheet name="screenTitles" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -114,18 +107,9 @@
     <t>"Proximus Light", ProximusLight</t>
   </si>
   <si>
-    <t>nitin</t>
-  </si>
-  <si>
-    <t>kaushik</t>
-  </si>
-  <si>
     <t>objectID</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>systeem</t>
   </si>
   <si>
@@ -139,6 +123,21 @@
   </si>
   <si>
     <t>HubMenu</t>
+  </si>
+  <si>
+    <t>epg</t>
+  </si>
+  <si>
+    <t>instellingen</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>epgSetting</t>
   </si>
 </sst>
 </file>
@@ -507,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,57 +528,57 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>85</v>
@@ -594,24 +593,24 @@
         <v>370</v>
       </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
         <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>365</v>
@@ -626,24 +625,24 @@
         <v>370</v>
       </c>
       <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" t="s">
         <v>16</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>531</v>
@@ -658,30 +657,30 @@
         <v>370</v>
       </c>
       <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
         <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="F5">
         <v>639</v>
@@ -690,10 +689,10 @@
         <v>560</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J5">
         <v>365</v>
@@ -702,27 +701,27 @@
         <v>370</v>
       </c>
       <c r="M5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F6">
         <v>729</v>
@@ -731,10 +730,10 @@
         <v>560</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J6">
         <v>365</v>
@@ -743,18 +742,18 @@
         <v>370</v>
       </c>
       <c r="M6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -778,99 +777,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>123</v>
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>